<commit_message>
working on integrating random_word
</commit_message>
<xml_diff>
--- a/wordle_plus_game/local_files/Score_Boards.xlsx
+++ b/wordle_plus_game/local_files/Score_Boards.xlsx
@@ -1,63 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytnstate-my.sharepoint.com/personal/afolorun_my_tnstate_edu/Documents/Technical/Personal Projects/WordGame/wordle_plus_game/local_files/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_7FD52E4030EF4E46C6B6321CE1EAB6D5F62BA245" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D05589C-A1C5-4B51-974C-8AC1BE71C946}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Top Scores" sheetId="1" r:id="rId1"/>
-    <sheet name="Classic" sheetId="2" r:id="rId2"/>
-    <sheet name="Hangman" sheetId="3" r:id="rId3"/>
+    <sheet name="Top Scores" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Classic" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Hangman" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
-  <si>
-    <t>Game mode</t>
-  </si>
-  <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -83,31 +61,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,50 +432,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col width="13.88671875" customWidth="1" min="1" max="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="1" min="3" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4"/>
-      <c r="D4"/>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Game mode</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Difficulty</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+    </row>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Classic</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>40</v>
+      </c>
+      <c r="D5" t="n">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -446,48 +507,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="1" min="2" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5"/>
-      <c r="C5"/>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Difficulty</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>40</v>
+      </c>
+      <c r="C6" t="n">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -495,9 +573,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -505,40 +584,43 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="1" min="2" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5"/>
-      <c r="C5"/>
-    </row>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Difficulty</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="B2" s="2" t="n"/>
+      <c r="C2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="n"/>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented Classic difficulty levels
</commit_message>
<xml_diff>
--- a/wordle_plus_game/local_files/Score_Boards.xlsx
+++ b/wordle_plus_game/local_files/Score_Boards.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,6 +523,42 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Classic</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>141</v>
+      </c>
+      <c r="D5" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Classic</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ultra Hard</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -534,7 +570,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,6 +650,45 @@
       </c>
       <c r="C5" t="n">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>141</v>
+      </c>
+      <c r="C6" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>211</v>
+      </c>
+      <c r="C7" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ultra Hard</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created basic working line graph, added to wordle classic
</commit_message>
<xml_diff>
--- a/wordle_plus_game/local_files/Score_Boards.xlsx
+++ b/wordle_plus_game/local_files/Score_Boards.xlsx
@@ -527,10 +527,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:C1"/>
@@ -696,6 +696,19 @@
         <v>19</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
desiign and function improvments
</commit_message>
<xml_diff>
--- a/wordle_plus_game/local_files/Score_Boards.xlsx
+++ b/wordle_plus_game/local_files/Score_Boards.xlsx
@@ -1,35 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytnstate-my.sharepoint.com/personal/afolorun_my_tnstate_edu/Documents/Technical/Techwise/WordGame/wordle_plus_game/local_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_F008AF42900F05855D9F4139DDF9E191CA8CC306" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{460EC40F-B8D1-4CC6-9A1C-0348E19F608E}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Top Scores" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Classic" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Hangman" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Top Scores" sheetId="1" r:id="rId1"/>
+    <sheet name="Classic" sheetId="2" r:id="rId2"/>
+    <sheet name="Hangman" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+  <si>
+    <t>Game mode</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Hangman</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,86 +89,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -422,114 +397,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="13.33203125" customWidth="1" min="1" max="1"/>
-    <col width="9.6640625" customWidth="1" min="2" max="3"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Game mode</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Difficulty</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Classic</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D2" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Hangman</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>21</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Classic</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Hard</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>43</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>14</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hangman</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Hard</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>58</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>19</v>
       </c>
     </row>
@@ -539,98 +486,133 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Difficulty</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>11</v>
       </c>
-      <c r="C2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>28</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>7</v>
-      </c>
-      <c r="C4" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>186</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>37</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Hard</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
         <v>43</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>186</v>
+      </c>
+      <c r="C10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>43</v>
+      </c>
+      <c r="C11">
         <v>14</v>
       </c>
     </row>
@@ -640,59 +622,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Difficulty</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>21</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Hard</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
         <v>58</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing variable call order
</commit_message>
<xml_diff>
--- a/wordle_plus_game/local_files/Score_Boards.xlsx
+++ b/wordle_plus_game/local_files/Score_Boards.xlsx
@@ -433,7 +433,7 @@
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="13.33203125" customWidth="1" min="1" max="1"/>
     <col width="9.6640625" customWidth="1" min="2" max="3"/>
@@ -645,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:C1"/>
@@ -696,6 +696,19 @@
         <v>19</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>457</v>
+      </c>
+      <c r="C4" t="n">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>